<commit_message>
Initial update with CPL’s work-to-date
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
+++ b/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariz\Desktop\Variáveis marianne FINAL\add-outputs\VoaSL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\add-outputs\VoaSL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BB40006-1E0B-41BE-BC97-64BDC5975A03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E59E064-EF61-4312-82D8-C31F8060157D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19308" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2310" yWindow="975" windowWidth="25830" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="VoaSL" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>VoaSL Value of a Statistical Life</t>
   </si>
@@ -39,12 +39,24 @@
     <t>Source:</t>
   </si>
   <si>
+    <t>U.S. Environmental Protection Agency</t>
+  </si>
+  <si>
+    <t>Frequently Asked Questions on Mortality Risk Valuation</t>
+  </si>
+  <si>
+    <t>We adjust 2006 dollars to 2012 dollars using the following conversion factor:</t>
+  </si>
+  <si>
     <t>See "cpi.xlsx" in the InputData folder for source information.</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
+    <t>"What value of statistical life does EPA use?"</t>
+  </si>
+  <si>
     <t>Statistical Life</t>
   </si>
   <si>
@@ -69,45 +81,14 @@
     <t>Value</t>
   </si>
   <si>
-    <t>IPEA</t>
-  </si>
-  <si>
-    <t>O CUSTO ECONÔMICO DA POLUIÇÃO DO AR: ESTIMATIVA DE VALOR DA VIDA ESTATÍSTICA PARA O BRASIL</t>
-  </si>
-  <si>
-    <t>http://www.ipea.gov.br/portal/index.php?option=com_content&amp;view=article&amp;id=35164</t>
-  </si>
-  <si>
-    <t>VSL pollution (average)=</t>
-  </si>
-  <si>
-    <t>millions (USD2017)</t>
-  </si>
-  <si>
-    <t>We adjust 2017 dollars to 2012 dollars using the following conversion factor:</t>
-  </si>
-  <si>
-    <r>
-      <t>("</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The economic cost of air pollution: an estimate of the value of a statistical life in Brazil")</t>
-    </r>
+    <t>https://www.epa.gov/environmental-economics/mortality-risk-valuation#whatvalue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,14 +108,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,7 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -172,10 +145,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -192,7 +164,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -512,113 +484,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <f>(0.69+1.24)/2</f>
-        <v>0.96499999999999997</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1.141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>0.93669999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" location="whatvalue" display="https://www.epa.gov/environmental-economics/mortality-risk-valuation - whatvalue" xr:uid="{F4EA8DF9-36E3-4A47-8B4C-6E99399B200A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -630,30 +591,30 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="6">
-        <f>About!C9*10^6*About!A18</f>
-        <v>903915.5</v>
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <f>7.4*10^6*About!A17</f>
+        <v>8443400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>